<commit_message>
added theme 7 and table
</commit_message>
<xml_diff>
--- a/OPD/Book1.xlsx
+++ b/OPD/Book1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Организационно-правовя форма</t>
   </si>
@@ -55,13 +55,34 @@
   </si>
   <si>
     <t xml:space="preserve">Всем своим имуществом в пределах устава</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фермерское хозяйство</t>
+  </si>
+  <si>
+    <t xml:space="preserve">от 1 и члены семьи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">По решению общего собрания</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В пределах вкладов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Открытой акционерное общество</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400 базовых величин</t>
+  </si>
+  <si>
+    <t xml:space="preserve">от 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -69,20 +90,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.000000"/>
+      <sz val="11.000000"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Courier New"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -91,16 +124,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color theme="1"/>
       </left>
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color theme="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color theme="1"/>
       </bottom>
       <diagonal/>
@@ -109,35 +142,34 @@
       <left style="thin">
         <color theme="1"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
         <color theme="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color theme="1"/>
       </left>
       <right/>
@@ -147,7 +179,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color theme="1"/>
       </right>
       <top/>
@@ -155,12 +187,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color theme="1"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color theme="1"/>
       </bottom>
       <diagonal/>
@@ -169,18 +201,18 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color theme="1"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color theme="1"/>
       </bottom>
       <diagonal/>
@@ -189,37 +221,34 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf fontId="2" fillId="2" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf fontId="2" fillId="2" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="3" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf fontId="2" fillId="2" borderId="3" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="4" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="5" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="6" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="7" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="8" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="9" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,9 +763,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="32.7109375"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="27.00390625"/>
+    <col customWidth="1" min="1" max="1" style="1" width="2.8515625"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="30.8828125"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="19.57421875"/>
     <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="25.8515625"/>
     <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="24.7109375"/>
     <col customWidth="1" min="6" max="6" style="1" width="24.00390625"/>
@@ -745,84 +774,135 @@
     <col min="9" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="2" ht="14.4">
+    <row r="1" ht="12" customHeight="1"/>
+    <row r="2" ht="28.5">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" ht="30.600000000000001" customHeight="1">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" ht="14.25">
-      <c r="B4" s="6"/>
-      <c r="H4" s="7"/>
+    <row r="4" ht="28.5">
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" ht="14.25">
-      <c r="B5" s="6"/>
-      <c r="H5" s="7"/>
+    <row r="5" ht="28.5">
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" ht="14.25">
-      <c r="B6" s="6"/>
-      <c r="H6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" ht="14.25">
-      <c r="B7" s="6"/>
-      <c r="H7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="B8" s="6"/>
-      <c r="H8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="B9" s="6"/>
-      <c r="H9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>